<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@c0870de5b4977f6807eba347ceb6b4d08fd46f4b 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-average-blood-pressure.xlsx
+++ b/StructureDefinition-us-core-average-blood-pressure.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AP$95</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3845" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3689" uniqueCount="619">
   <si>
     <t>Property</t>
   </si>
@@ -1716,19 +1716,6 @@
     <t>Observation.component:systolic.value[x]</t>
   </si>
   <si>
-    <t>Actual component result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>Observation.component:systolic.value[x]:valueQuantity</t>
-  </si>
-  <si>
-    <t>valueQuantity</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quantity
 </t>
   </si>
@@ -1740,19 +1727,19 @@
 </t>
   </si>
   <si>
-    <t>Observation.component:systolic.value[x]:valueQuantity.id</t>
+    <t>Observation.component:systolic.value[x].id</t>
   </si>
   <si>
     <t>Observation.component.value[x].id</t>
   </si>
   <si>
-    <t>Observation.component:systolic.value[x]:valueQuantity.extension</t>
+    <t>Observation.component:systolic.value[x].extension</t>
   </si>
   <si>
     <t>Observation.component.value[x].extension</t>
   </si>
   <si>
-    <t>Observation.component:systolic.value[x]:valueQuantity.value</t>
+    <t>Observation.component:systolic.value[x].value</t>
   </si>
   <si>
     <t>Observation.component.value[x].value</t>
@@ -1783,7 +1770,7 @@
     <t>PQ.value, CO.value, MO.value, IVL.high or IVL.low depending on the value</t>
   </si>
   <si>
-    <t>Observation.component:systolic.value[x]:valueQuantity.comparator</t>
+    <t>Observation.component:systolic.value[x].comparator</t>
   </si>
   <si>
     <t>Observation.component.value[x].comparator</t>
@@ -1816,7 +1803,7 @@
     <t>IVL properties</t>
   </si>
   <si>
-    <t>Observation.component:systolic.value[x]:valueQuantity.unit</t>
+    <t>Observation.component:systolic.value[x].unit</t>
   </si>
   <si>
     <t>Observation.component.value[x].unit</t>
@@ -1840,7 +1827,7 @@
     <t>PQ.unit</t>
   </si>
   <si>
-    <t>Observation.component:systolic.value[x]:valueQuantity.system</t>
+    <t>Observation.component:systolic.value[x].system</t>
   </si>
   <si>
     <t>Observation.component.value[x].system</t>
@@ -1868,7 +1855,7 @@
     <t>CO.codeSystem, PQ.translation.codeSystem</t>
   </si>
   <si>
-    <t>Observation.component:systolic.value[x]:valueQuantity.code</t>
+    <t>Observation.component:systolic.value[x].code</t>
   </si>
   <si>
     <t>Observation.component.value[x].code</t>
@@ -1939,31 +1926,28 @@
     <t>Observation.component:diastolic.value[x]</t>
   </si>
   <si>
-    <t>Observation.component:diastolic.value[x]:valueQuantity</t>
-  </si>
-  <si>
     <t>Diastolic Average Blood Pressure Value</t>
   </si>
   <si>
-    <t>Observation.component:diastolic.value[x]:valueQuantity.id</t>
-  </si>
-  <si>
-    <t>Observation.component:diastolic.value[x]:valueQuantity.extension</t>
-  </si>
-  <si>
-    <t>Observation.component:diastolic.value[x]:valueQuantity.value</t>
-  </si>
-  <si>
-    <t>Observation.component:diastolic.value[x]:valueQuantity.comparator</t>
-  </si>
-  <si>
-    <t>Observation.component:diastolic.value[x]:valueQuantity.unit</t>
-  </si>
-  <si>
-    <t>Observation.component:diastolic.value[x]:valueQuantity.system</t>
-  </si>
-  <si>
-    <t>Observation.component:diastolic.value[x]:valueQuantity.code</t>
+    <t>Observation.component:diastolic.value[x].id</t>
+  </si>
+  <si>
+    <t>Observation.component:diastolic.value[x].extension</t>
+  </si>
+  <si>
+    <t>Observation.component:diastolic.value[x].value</t>
+  </si>
+  <si>
+    <t>Observation.component:diastolic.value[x].comparator</t>
+  </si>
+  <si>
+    <t>Observation.component:diastolic.value[x].unit</t>
+  </si>
+  <si>
+    <t>Observation.component:diastolic.value[x].system</t>
+  </si>
+  <si>
+    <t>Observation.component:diastolic.value[x].code</t>
   </si>
   <si>
     <t>Observation.component:diastolic.dataAbsentReason</t>
@@ -2294,7 +2278,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AP99"/>
+  <dimension ref="A1:AP95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -2303,9 +2287,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="55.1328125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="43.51953125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="38.30078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.98046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="34.21875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
@@ -10577,7 +10561,7 @@
         <v>92</v>
       </c>
       <c r="H69" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I69" t="s" s="2">
         <v>82</v>
@@ -10586,13 +10570,13 @@
         <v>93</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>356</v>
+        <v>541</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>358</v>
+        <v>519</v>
       </c>
       <c r="N69" t="s" s="2">
         <v>520</v>
@@ -10635,14 +10619,16 @@
         <v>82</v>
       </c>
       <c r="AB69" t="s" s="2">
-        <v>542</v>
-      </c>
-      <c r="AC69" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>82</v>
+      </c>
       <c r="AD69" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>198</v>
+        <v>82</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>517</v>
@@ -10654,7 +10640,7 @@
         <v>92</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>82</v>
+        <v>543</v>
       </c>
       <c r="AJ69" t="s" s="2">
         <v>104</v>
@@ -10680,14 +10666,12 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>517</v>
-      </c>
-      <c r="C70" t="s" s="2">
-        <v>544</v>
-      </c>
+        <v>545</v>
+      </c>
+      <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
         <v>82</v>
       </c>
@@ -10699,29 +10683,25 @@
         <v>92</v>
       </c>
       <c r="H70" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I70" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J70" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>545</v>
+        <v>205</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>546</v>
+        <v>206</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>520</v>
-      </c>
-      <c r="O70" t="s" s="2">
-        <v>360</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
       <c r="P70" t="s" s="2">
         <v>82</v>
       </c>
@@ -10769,7 +10749,7 @@
         <v>82</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>517</v>
+        <v>208</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>80</v>
@@ -10778,47 +10758,47 @@
         <v>92</v>
       </c>
       <c r="AI70" t="s" s="2">
-        <v>547</v>
+        <v>82</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="AK70" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>521</v>
+        <v>82</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>363</v>
+        <v>82</v>
       </c>
       <c r="AN70" t="s" s="2">
-        <v>364</v>
+        <v>209</v>
       </c>
       <c r="AO70" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP70" t="s" s="2">
-        <v>365</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
-        <v>82</v>
+        <v>137</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G71" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H71" t="s" s="2">
         <v>82</v>
@@ -10830,15 +10810,17 @@
         <v>82</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>206</v>
+        <v>139</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="N71" s="2"/>
+        <v>212</v>
+      </c>
+      <c r="N71" t="s" s="2">
+        <v>141</v>
+      </c>
       <c r="O71" s="2"/>
       <c r="P71" t="s" s="2">
         <v>82</v>
@@ -10875,31 +10857,31 @@
         <v>82</v>
       </c>
       <c r="AB71" t="s" s="2">
-        <v>82</v>
+        <v>213</v>
       </c>
       <c r="AC71" t="s" s="2">
-        <v>82</v>
+        <v>214</v>
       </c>
       <c r="AD71" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>82</v>
+        <v>198</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH71" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI71" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="AK71" t="s" s="2">
         <v>82</v>
@@ -10922,21 +10904,21 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="E72" s="2"/>
       <c r="F72" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G72" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H72" t="s" s="2">
         <v>82</v>
@@ -10945,21 +10927,23 @@
         <v>82</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>138</v>
+        <v>550</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>139</v>
+        <v>551</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>212</v>
+        <v>552</v>
       </c>
       <c r="N72" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O72" s="2"/>
+        <v>553</v>
+      </c>
+      <c r="O72" t="s" s="2">
+        <v>554</v>
+      </c>
       <c r="P72" t="s" s="2">
         <v>82</v>
       </c>
@@ -10995,31 +10979,31 @@
         <v>82</v>
       </c>
       <c r="AB72" t="s" s="2">
-        <v>213</v>
+        <v>82</v>
       </c>
       <c r="AC72" t="s" s="2">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="AD72" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>198</v>
+        <v>82</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>215</v>
+        <v>555</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH72" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI72" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="AK72" t="s" s="2">
         <v>82</v>
@@ -11028,10 +11012,10 @@
         <v>82</v>
       </c>
       <c r="AM72" t="s" s="2">
-        <v>82</v>
+        <v>556</v>
       </c>
       <c r="AN72" t="s" s="2">
-        <v>209</v>
+        <v>557</v>
       </c>
       <c r="AO72" t="s" s="2">
         <v>82</v>
@@ -11042,10 +11026,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -11053,7 +11037,7 @@
       </c>
       <c r="E73" s="2"/>
       <c r="F73" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G73" t="s" s="2">
         <v>92</v>
@@ -11062,30 +11046,30 @@
         <v>82</v>
       </c>
       <c r="I73" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="J73" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>554</v>
+        <v>112</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>556</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>557</v>
-      </c>
+        <v>561</v>
+      </c>
+      <c r="N73" s="2"/>
       <c r="O73" t="s" s="2">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="P73" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="Q73" s="2"/>
+      <c r="Q73" t="s" s="2">
+        <v>563</v>
+      </c>
       <c r="R73" t="s" s="2">
         <v>82</v>
       </c>
@@ -11105,13 +11089,13 @@
         <v>82</v>
       </c>
       <c r="X73" t="s" s="2">
-        <v>82</v>
+        <v>181</v>
       </c>
       <c r="Y73" t="s" s="2">
-        <v>82</v>
+        <v>564</v>
       </c>
       <c r="Z73" t="s" s="2">
-        <v>82</v>
+        <v>565</v>
       </c>
       <c r="AA73" t="s" s="2">
         <v>82</v>
@@ -11129,7 +11113,7 @@
         <v>82</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>80</v>
@@ -11150,10 +11134,10 @@
         <v>82</v>
       </c>
       <c r="AM73" t="s" s="2">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="AN73" t="s" s="2">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="AO73" t="s" s="2">
         <v>82</v>
@@ -11164,10 +11148,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>563</v>
+        <v>570</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -11175,7 +11159,7 @@
       </c>
       <c r="E74" s="2"/>
       <c r="F74" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G74" t="s" s="2">
         <v>92</v>
@@ -11184,30 +11168,28 @@
         <v>82</v>
       </c>
       <c r="I74" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="J74" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>112</v>
+        <v>205</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="P74" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="Q74" t="s" s="2">
-        <v>567</v>
-      </c>
+      <c r="Q74" s="2"/>
       <c r="R74" t="s" s="2">
         <v>82</v>
       </c>
@@ -11227,13 +11209,13 @@
         <v>82</v>
       </c>
       <c r="X74" t="s" s="2">
-        <v>181</v>
+        <v>82</v>
       </c>
       <c r="Y74" t="s" s="2">
-        <v>568</v>
+        <v>82</v>
       </c>
       <c r="Z74" t="s" s="2">
-        <v>569</v>
+        <v>82</v>
       </c>
       <c r="AA74" t="s" s="2">
         <v>82</v>
@@ -11251,7 +11233,7 @@
         <v>82</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>80</v>
@@ -11272,10 +11254,10 @@
         <v>82</v>
       </c>
       <c r="AM74" t="s" s="2">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="AN74" t="s" s="2">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="AO74" t="s" s="2">
         <v>82</v>
@@ -11286,10 +11268,10 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -11312,24 +11294,24 @@
         <v>93</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>205</v>
+        <v>106</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="P75" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q75" s="2"/>
       <c r="R75" t="s" s="2">
-        <v>82</v>
+        <v>582</v>
       </c>
       <c r="S75" t="s" s="2">
         <v>82</v>
@@ -11371,7 +11353,7 @@
         <v>82</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>80</v>
@@ -11380,7 +11362,7 @@
         <v>92</v>
       </c>
       <c r="AI75" t="s" s="2">
-        <v>82</v>
+        <v>584</v>
       </c>
       <c r="AJ75" t="s" s="2">
         <v>104</v>
@@ -11392,10 +11374,10 @@
         <v>82</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="AN75" t="s" s="2">
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="AO75" t="s" s="2">
         <v>82</v>
@@ -11406,10 +11388,10 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>581</v>
+        <v>586</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -11432,24 +11414,26 @@
         <v>93</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>583</v>
+        <v>588</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>584</v>
-      </c>
-      <c r="N76" s="2"/>
+        <v>589</v>
+      </c>
+      <c r="N76" t="s" s="2">
+        <v>590</v>
+      </c>
       <c r="O76" t="s" s="2">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c r="P76" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q76" s="2"/>
       <c r="R76" t="s" s="2">
-        <v>586</v>
+        <v>592</v>
       </c>
       <c r="S76" t="s" s="2">
         <v>82</v>
@@ -11491,7 +11475,7 @@
         <v>82</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>587</v>
+        <v>593</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>80</v>
@@ -11500,7 +11484,7 @@
         <v>92</v>
       </c>
       <c r="AI76" t="s" s="2">
-        <v>588</v>
+        <v>82</v>
       </c>
       <c r="AJ76" t="s" s="2">
         <v>104</v>
@@ -11512,10 +11496,10 @@
         <v>82</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="AN76" t="s" s="2">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="AO76" t="s" s="2">
         <v>82</v>
@@ -11526,10 +11510,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>591</v>
+        <v>522</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -11537,41 +11521,41 @@
       </c>
       <c r="E77" s="2"/>
       <c r="F77" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G77" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H77" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I77" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>112</v>
+        <v>190</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>592</v>
+        <v>523</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>593</v>
+        <v>524</v>
       </c>
       <c r="N77" t="s" s="2">
-        <v>594</v>
+        <v>525</v>
       </c>
       <c r="O77" t="s" s="2">
-        <v>595</v>
+        <v>370</v>
       </c>
       <c r="P77" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q77" s="2"/>
       <c r="R77" t="s" s="2">
-        <v>596</v>
+        <v>82</v>
       </c>
       <c r="S77" t="s" s="2">
         <v>82</v>
@@ -11589,13 +11573,13 @@
         <v>82</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>82</v>
+        <v>371</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>82</v>
+        <v>372</v>
       </c>
       <c r="Z77" t="s" s="2">
-        <v>82</v>
+        <v>373</v>
       </c>
       <c r="AA77" t="s" s="2">
         <v>82</v>
@@ -11613,7 +11597,7 @@
         <v>82</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>597</v>
+        <v>522</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>80</v>
@@ -11622,7 +11606,7 @@
         <v>92</v>
       </c>
       <c r="AI77" t="s" s="2">
-        <v>82</v>
+        <v>526</v>
       </c>
       <c r="AJ77" t="s" s="2">
         <v>104</v>
@@ -11634,10 +11618,10 @@
         <v>82</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>579</v>
+        <v>135</v>
       </c>
       <c r="AN77" t="s" s="2">
-        <v>598</v>
+        <v>375</v>
       </c>
       <c r="AO77" t="s" s="2">
         <v>82</v>
@@ -11648,45 +11632,45 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>540</v>
+        <v>596</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>517</v>
+        <v>527</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
-        <v>82</v>
+        <v>377</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H78" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I78" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J78" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>356</v>
+        <v>190</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>518</v>
+        <v>378</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>519</v>
+        <v>379</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>520</v>
+        <v>380</v>
       </c>
       <c r="O78" t="s" s="2">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="P78" t="s" s="2">
         <v>82</v>
@@ -11711,13 +11695,13 @@
         <v>82</v>
       </c>
       <c r="X78" t="s" s="2">
-        <v>82</v>
+        <v>371</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>82</v>
+        <v>382</v>
       </c>
       <c r="Z78" t="s" s="2">
-        <v>82</v>
+        <v>383</v>
       </c>
       <c r="AA78" t="s" s="2">
         <v>82</v>
@@ -11735,13 +11719,13 @@
         <v>82</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>517</v>
+        <v>527</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH78" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI78" t="s" s="2">
         <v>82</v>
@@ -11753,27 +11737,27 @@
         <v>82</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>521</v>
+        <v>384</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>363</v>
+        <v>385</v>
       </c>
       <c r="AN78" t="s" s="2">
-        <v>364</v>
+        <v>386</v>
       </c>
       <c r="AO78" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP78" t="s" s="2">
-        <v>365</v>
+        <v>387</v>
       </c>
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11784,10 +11768,10 @@
         <v>80</v>
       </c>
       <c r="G79" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H79" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I79" t="s" s="2">
         <v>82</v>
@@ -11796,19 +11780,19 @@
         <v>82</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>190</v>
+        <v>83</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>525</v>
+        <v>437</v>
       </c>
       <c r="O79" t="s" s="2">
-        <v>370</v>
+        <v>438</v>
       </c>
       <c r="P79" t="s" s="2">
         <v>82</v>
@@ -11833,13 +11817,13 @@
         <v>82</v>
       </c>
       <c r="X79" t="s" s="2">
-        <v>371</v>
+        <v>82</v>
       </c>
       <c r="Y79" t="s" s="2">
-        <v>372</v>
+        <v>82</v>
       </c>
       <c r="Z79" t="s" s="2">
-        <v>373</v>
+        <v>82</v>
       </c>
       <c r="AA79" t="s" s="2">
         <v>82</v>
@@ -11857,16 +11841,16 @@
         <v>82</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH79" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI79" t="s" s="2">
-        <v>526</v>
+        <v>82</v>
       </c>
       <c r="AJ79" t="s" s="2">
         <v>104</v>
@@ -11878,10 +11862,10 @@
         <v>82</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>135</v>
+        <v>440</v>
       </c>
       <c r="AN79" t="s" s="2">
-        <v>375</v>
+        <v>441</v>
       </c>
       <c r="AO79" t="s" s="2">
         <v>82</v>
@@ -11892,45 +11876,47 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>527</v>
-      </c>
-      <c r="C80" s="2"/>
+        <v>499</v>
+      </c>
+      <c r="C80" t="s" s="2">
+        <v>599</v>
+      </c>
       <c r="D80" t="s" s="2">
-        <v>377</v>
+        <v>82</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G80" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H80" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I80" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>190</v>
+        <v>434</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>378</v>
+        <v>600</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>379</v>
+        <v>502</v>
       </c>
       <c r="N80" t="s" s="2">
-        <v>380</v>
+        <v>503</v>
       </c>
       <c r="O80" t="s" s="2">
-        <v>381</v>
+        <v>504</v>
       </c>
       <c r="P80" t="s" s="2">
         <v>82</v>
@@ -11955,13 +11941,13 @@
         <v>82</v>
       </c>
       <c r="X80" t="s" s="2">
-        <v>371</v>
+        <v>82</v>
       </c>
       <c r="Y80" t="s" s="2">
-        <v>382</v>
+        <v>82</v>
       </c>
       <c r="Z80" t="s" s="2">
-        <v>383</v>
+        <v>82</v>
       </c>
       <c r="AA80" t="s" s="2">
         <v>82</v>
@@ -11979,7 +11965,7 @@
         <v>82</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>527</v>
+        <v>499</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>80</v>
@@ -11997,19 +11983,19 @@
         <v>82</v>
       </c>
       <c r="AL80" t="s" s="2">
-        <v>384</v>
+        <v>82</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>385</v>
+        <v>507</v>
       </c>
       <c r="AN80" t="s" s="2">
-        <v>386</v>
+        <v>508</v>
       </c>
       <c r="AO80" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP80" t="s" s="2">
-        <v>387</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" hidden="true">
@@ -12017,7 +12003,7 @@
         <v>601</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>528</v>
+        <v>509</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -12028,7 +12014,7 @@
         <v>80</v>
       </c>
       <c r="G81" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H81" t="s" s="2">
         <v>82</v>
@@ -12040,20 +12026,16 @@
         <v>82</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>83</v>
+        <v>205</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>529</v>
+        <v>206</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>530</v>
-      </c>
-      <c r="N81" t="s" s="2">
-        <v>437</v>
-      </c>
-      <c r="O81" t="s" s="2">
-        <v>438</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="N81" s="2"/>
+      <c r="O81" s="2"/>
       <c r="P81" t="s" s="2">
         <v>82</v>
       </c>
@@ -12101,19 +12083,19 @@
         <v>82</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>528</v>
+        <v>208</v>
       </c>
       <c r="AG81" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI81" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="AK81" t="s" s="2">
         <v>82</v>
@@ -12122,10 +12104,10 @@
         <v>82</v>
       </c>
       <c r="AM81" t="s" s="2">
-        <v>440</v>
+        <v>82</v>
       </c>
       <c r="AN81" t="s" s="2">
-        <v>441</v>
+        <v>209</v>
       </c>
       <c r="AO81" t="s" s="2">
         <v>82</v>
@@ -12139,45 +12121,41 @@
         <v>602</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>499</v>
-      </c>
-      <c r="C82" t="s" s="2">
-        <v>603</v>
-      </c>
+        <v>510</v>
+      </c>
+      <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
-        <v>82</v>
+        <v>137</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G82" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H82" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I82" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>434</v>
+        <v>138</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>604</v>
+        <v>139</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>502</v>
+        <v>212</v>
       </c>
       <c r="N82" t="s" s="2">
-        <v>503</v>
-      </c>
-      <c r="O82" t="s" s="2">
-        <v>504</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="O82" s="2"/>
       <c r="P82" t="s" s="2">
         <v>82</v>
       </c>
@@ -12225,7 +12203,7 @@
         <v>82</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>499</v>
+        <v>215</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>80</v>
@@ -12237,7 +12215,7 @@
         <v>82</v>
       </c>
       <c r="AJ82" t="s" s="2">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="AK82" t="s" s="2">
         <v>82</v>
@@ -12246,10 +12224,10 @@
         <v>82</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>507</v>
+        <v>82</v>
       </c>
       <c r="AN82" t="s" s="2">
-        <v>508</v>
+        <v>209</v>
       </c>
       <c r="AO82" t="s" s="2">
         <v>82</v>
@@ -12260,42 +12238,46 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
-        <v>82</v>
+        <v>445</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G83" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H83" t="s" s="2">
         <v>82</v>
       </c>
       <c r="I83" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>206</v>
+        <v>446</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="N83" s="2"/>
-      <c r="O83" s="2"/>
+        <v>447</v>
+      </c>
+      <c r="N83" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="O83" t="s" s="2">
+        <v>147</v>
+      </c>
       <c r="P83" t="s" s="2">
         <v>82</v>
       </c>
@@ -12343,19 +12325,19 @@
         <v>82</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>208</v>
+        <v>448</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH83" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI83" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>82</v>
+        <v>143</v>
       </c>
       <c r="AK83" t="s" s="2">
         <v>82</v>
@@ -12367,7 +12349,7 @@
         <v>82</v>
       </c>
       <c r="AN83" t="s" s="2">
-        <v>209</v>
+        <v>135</v>
       </c>
       <c r="AO83" t="s" s="2">
         <v>82</v>
@@ -12378,44 +12360,46 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G84" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H84" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I84" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>138</v>
+        <v>190</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>139</v>
+        <v>605</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>212</v>
+        <v>514</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O84" s="2"/>
+        <v>515</v>
+      </c>
+      <c r="O84" t="s" s="2">
+        <v>289</v>
+      </c>
       <c r="P84" t="s" s="2">
         <v>82</v>
       </c>
@@ -12424,7 +12408,7 @@
         <v>82</v>
       </c>
       <c r="S84" t="s" s="2">
-        <v>82</v>
+        <v>606</v>
       </c>
       <c r="T84" t="s" s="2">
         <v>82</v>
@@ -12439,13 +12423,13 @@
         <v>82</v>
       </c>
       <c r="X84" t="s" s="2">
-        <v>82</v>
+        <v>291</v>
       </c>
       <c r="Y84" t="s" s="2">
-        <v>82</v>
+        <v>292</v>
       </c>
       <c r="Z84" t="s" s="2">
-        <v>82</v>
+        <v>293</v>
       </c>
       <c r="AA84" t="s" s="2">
         <v>82</v>
@@ -12463,34 +12447,34 @@
         <v>82</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>215</v>
+        <v>512</v>
       </c>
       <c r="AG84" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="AH84" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI84" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="AK84" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL84" t="s" s="2">
-        <v>82</v>
+        <v>516</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>82</v>
+        <v>296</v>
       </c>
       <c r="AN84" t="s" s="2">
-        <v>209</v>
+        <v>297</v>
       </c>
       <c r="AO84" t="s" s="2">
-        <v>82</v>
+        <v>298</v>
       </c>
       <c r="AP84" t="s" s="2">
         <v>82</v>
@@ -12501,42 +12485,42 @@
         <v>607</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
-        <v>445</v>
+        <v>82</v>
       </c>
       <c r="E85" s="2"/>
       <c r="F85" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G85" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H85" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I85" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="J85" t="s" s="2">
         <v>93</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>138</v>
+        <v>541</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>446</v>
+        <v>608</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>447</v>
+        <v>519</v>
       </c>
       <c r="N85" t="s" s="2">
-        <v>141</v>
+        <v>520</v>
       </c>
       <c r="O85" t="s" s="2">
-        <v>147</v>
+        <v>360</v>
       </c>
       <c r="P85" t="s" s="2">
         <v>82</v>
@@ -12585,45 +12569,45 @@
         <v>82</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>448</v>
+        <v>517</v>
       </c>
       <c r="AG85" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH85" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI85" t="s" s="2">
-        <v>82</v>
+        <v>543</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="AK85" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>82</v>
+        <v>521</v>
       </c>
       <c r="AM85" t="s" s="2">
-        <v>82</v>
+        <v>363</v>
       </c>
       <c r="AN85" t="s" s="2">
-        <v>135</v>
+        <v>364</v>
       </c>
       <c r="AO85" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP85" t="s" s="2">
-        <v>82</v>
+        <v>365</v>
       </c>
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>512</v>
+        <v>545</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12631,35 +12615,31 @@
       </c>
       <c r="E86" s="2"/>
       <c r="F86" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G86" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H86" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I86" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J86" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>609</v>
+        <v>206</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>514</v>
-      </c>
-      <c r="N86" t="s" s="2">
-        <v>515</v>
-      </c>
-      <c r="O86" t="s" s="2">
-        <v>289</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="N86" s="2"/>
+      <c r="O86" s="2"/>
       <c r="P86" t="s" s="2">
         <v>82</v>
       </c>
@@ -12668,7 +12648,7 @@
         <v>82</v>
       </c>
       <c r="S86" t="s" s="2">
-        <v>610</v>
+        <v>82</v>
       </c>
       <c r="T86" t="s" s="2">
         <v>82</v>
@@ -12683,13 +12663,13 @@
         <v>82</v>
       </c>
       <c r="X86" t="s" s="2">
-        <v>291</v>
+        <v>82</v>
       </c>
       <c r="Y86" t="s" s="2">
-        <v>292</v>
+        <v>82</v>
       </c>
       <c r="Z86" t="s" s="2">
-        <v>293</v>
+        <v>82</v>
       </c>
       <c r="AA86" t="s" s="2">
         <v>82</v>
@@ -12707,10 +12687,10 @@
         <v>82</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>512</v>
+        <v>208</v>
       </c>
       <c r="AG86" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="AH86" t="s" s="2">
         <v>92</v>
@@ -12719,22 +12699,22 @@
         <v>82</v>
       </c>
       <c r="AJ86" t="s" s="2">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="AK86" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>516</v>
+        <v>82</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>296</v>
+        <v>82</v>
       </c>
       <c r="AN86" t="s" s="2">
-        <v>297</v>
+        <v>209</v>
       </c>
       <c r="AO86" t="s" s="2">
-        <v>298</v>
+        <v>82</v>
       </c>
       <c r="AP86" t="s" s="2">
         <v>82</v>
@@ -12742,21 +12722,21 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>517</v>
+        <v>547</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
-        <v>82</v>
+        <v>137</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" t="s" s="2">
         <v>80</v>
       </c>
       <c r="G87" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H87" t="s" s="2">
         <v>82</v>
@@ -12765,23 +12745,21 @@
         <v>82</v>
       </c>
       <c r="J87" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>356</v>
+        <v>138</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>541</v>
+        <v>139</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>358</v>
+        <v>212</v>
       </c>
       <c r="N87" t="s" s="2">
-        <v>520</v>
-      </c>
-      <c r="O87" t="s" s="2">
-        <v>360</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="O87" s="2"/>
       <c r="P87" t="s" s="2">
         <v>82</v>
       </c>
@@ -12817,9 +12795,11 @@
         <v>82</v>
       </c>
       <c r="AB87" t="s" s="2">
-        <v>542</v>
-      </c>
-      <c r="AC87" s="2"/>
+        <v>213</v>
+      </c>
+      <c r="AC87" t="s" s="2">
+        <v>214</v>
+      </c>
       <c r="AD87" t="s" s="2">
         <v>82</v>
       </c>
@@ -12827,61 +12807,59 @@
         <v>198</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>517</v>
+        <v>215</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH87" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI87" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AJ87" t="s" s="2">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="AK87" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AL87" t="s" s="2">
-        <v>521</v>
+        <v>82</v>
       </c>
       <c r="AM87" t="s" s="2">
-        <v>363</v>
+        <v>82</v>
       </c>
       <c r="AN87" t="s" s="2">
-        <v>364</v>
+        <v>209</v>
       </c>
       <c r="AO87" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP87" t="s" s="2">
-        <v>365</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>517</v>
-      </c>
-      <c r="C88" t="s" s="2">
-        <v>544</v>
-      </c>
+        <v>549</v>
+      </c>
+      <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
         <v>82</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G88" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H88" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I88" t="s" s="2">
         <v>82</v>
@@ -12890,19 +12868,19 @@
         <v>93</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>613</v>
+        <v>551</v>
       </c>
       <c r="M88" t="s" s="2">
-        <v>358</v>
+        <v>552</v>
       </c>
       <c r="N88" t="s" s="2">
-        <v>520</v>
+        <v>553</v>
       </c>
       <c r="O88" t="s" s="2">
-        <v>360</v>
+        <v>554</v>
       </c>
       <c r="P88" t="s" s="2">
         <v>82</v>
@@ -12951,7 +12929,7 @@
         <v>82</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>517</v>
+        <v>555</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>80</v>
@@ -12960,7 +12938,7 @@
         <v>92</v>
       </c>
       <c r="AI88" t="s" s="2">
-        <v>547</v>
+        <v>82</v>
       </c>
       <c r="AJ88" t="s" s="2">
         <v>104</v>
@@ -12969,27 +12947,27 @@
         <v>82</v>
       </c>
       <c r="AL88" t="s" s="2">
-        <v>521</v>
+        <v>82</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>363</v>
+        <v>556</v>
       </c>
       <c r="AN88" t="s" s="2">
-        <v>364</v>
+        <v>557</v>
       </c>
       <c r="AO88" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP88" t="s" s="2">
-        <v>365</v>
+        <v>82</v>
       </c>
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>549</v>
+        <v>559</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
@@ -13006,26 +12984,30 @@
         <v>82</v>
       </c>
       <c r="I89" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="J89" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K89" t="s" s="2">
-        <v>205</v>
+        <v>112</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>206</v>
+        <v>560</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>207</v>
+        <v>561</v>
       </c>
       <c r="N89" s="2"/>
-      <c r="O89" s="2"/>
+      <c r="O89" t="s" s="2">
+        <v>562</v>
+      </c>
       <c r="P89" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="Q89" s="2"/>
+      <c r="Q89" t="s" s="2">
+        <v>563</v>
+      </c>
       <c r="R89" t="s" s="2">
         <v>82</v>
       </c>
@@ -13045,13 +13027,13 @@
         <v>82</v>
       </c>
       <c r="X89" t="s" s="2">
-        <v>82</v>
+        <v>181</v>
       </c>
       <c r="Y89" t="s" s="2">
-        <v>82</v>
+        <v>564</v>
       </c>
       <c r="Z89" t="s" s="2">
-        <v>82</v>
+        <v>565</v>
       </c>
       <c r="AA89" t="s" s="2">
         <v>82</v>
@@ -13069,7 +13051,7 @@
         <v>82</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>208</v>
+        <v>566</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>80</v>
@@ -13081,7 +13063,7 @@
         <v>82</v>
       </c>
       <c r="AJ89" t="s" s="2">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="AK89" t="s" s="2">
         <v>82</v>
@@ -13090,10 +13072,10 @@
         <v>82</v>
       </c>
       <c r="AM89" t="s" s="2">
-        <v>82</v>
+        <v>567</v>
       </c>
       <c r="AN89" t="s" s="2">
-        <v>209</v>
+        <v>568</v>
       </c>
       <c r="AO89" t="s" s="2">
         <v>82</v>
@@ -13104,21 +13086,21 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>551</v>
+        <v>570</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
-        <v>137</v>
+        <v>82</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G90" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="H90" t="s" s="2">
         <v>82</v>
@@ -13127,21 +13109,21 @@
         <v>82</v>
       </c>
       <c r="J90" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>138</v>
+        <v>205</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>139</v>
+        <v>571</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="N90" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O90" s="2"/>
+        <v>572</v>
+      </c>
+      <c r="N90" s="2"/>
+      <c r="O90" t="s" s="2">
+        <v>573</v>
+      </c>
       <c r="P90" t="s" s="2">
         <v>82</v>
       </c>
@@ -13177,31 +13159,31 @@
         <v>82</v>
       </c>
       <c r="AB90" t="s" s="2">
-        <v>213</v>
+        <v>82</v>
       </c>
       <c r="AC90" t="s" s="2">
-        <v>214</v>
+        <v>82</v>
       </c>
       <c r="AD90" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>198</v>
+        <v>82</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>215</v>
+        <v>574</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH90" t="s" s="2">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="AI90" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AJ90" t="s" s="2">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="AK90" t="s" s="2">
         <v>82</v>
@@ -13210,10 +13192,10 @@
         <v>82</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>82</v>
+        <v>575</v>
       </c>
       <c r="AN90" t="s" s="2">
-        <v>209</v>
+        <v>576</v>
       </c>
       <c r="AO90" t="s" s="2">
         <v>82</v>
@@ -13224,10 +13206,10 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>553</v>
+        <v>578</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -13250,26 +13232,24 @@
         <v>93</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>554</v>
+        <v>106</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>555</v>
+        <v>579</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>556</v>
-      </c>
-      <c r="N91" t="s" s="2">
-        <v>557</v>
-      </c>
+        <v>580</v>
+      </c>
+      <c r="N91" s="2"/>
       <c r="O91" t="s" s="2">
-        <v>558</v>
+        <v>581</v>
       </c>
       <c r="P91" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q91" s="2"/>
       <c r="R91" t="s" s="2">
-        <v>82</v>
+        <v>582</v>
       </c>
       <c r="S91" t="s" s="2">
         <v>82</v>
@@ -13311,7 +13291,7 @@
         <v>82</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>559</v>
+        <v>583</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>80</v>
@@ -13320,7 +13300,7 @@
         <v>92</v>
       </c>
       <c r="AI91" t="s" s="2">
-        <v>82</v>
+        <v>584</v>
       </c>
       <c r="AJ91" t="s" s="2">
         <v>104</v>
@@ -13332,10 +13312,10 @@
         <v>82</v>
       </c>
       <c r="AM91" t="s" s="2">
-        <v>560</v>
+        <v>575</v>
       </c>
       <c r="AN91" t="s" s="2">
-        <v>561</v>
+        <v>585</v>
       </c>
       <c r="AO91" t="s" s="2">
         <v>82</v>
@@ -13346,10 +13326,10 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>563</v>
+        <v>587</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
@@ -13357,7 +13337,7 @@
       </c>
       <c r="E92" s="2"/>
       <c r="F92" t="s" s="2">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="G92" t="s" s="2">
         <v>92</v>
@@ -13366,7 +13346,7 @@
         <v>82</v>
       </c>
       <c r="I92" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="J92" t="s" s="2">
         <v>93</v>
@@ -13375,23 +13355,23 @@
         <v>112</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>564</v>
+        <v>588</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>565</v>
-      </c>
-      <c r="N92" s="2"/>
+        <v>589</v>
+      </c>
+      <c r="N92" t="s" s="2">
+        <v>590</v>
+      </c>
       <c r="O92" t="s" s="2">
-        <v>566</v>
+        <v>591</v>
       </c>
       <c r="P92" t="s" s="2">
         <v>82</v>
       </c>
-      <c r="Q92" t="s" s="2">
-        <v>567</v>
-      </c>
+      <c r="Q92" s="2"/>
       <c r="R92" t="s" s="2">
-        <v>82</v>
+        <v>592</v>
       </c>
       <c r="S92" t="s" s="2">
         <v>82</v>
@@ -13409,13 +13389,13 @@
         <v>82</v>
       </c>
       <c r="X92" t="s" s="2">
-        <v>181</v>
+        <v>82</v>
       </c>
       <c r="Y92" t="s" s="2">
-        <v>568</v>
+        <v>82</v>
       </c>
       <c r="Z92" t="s" s="2">
-        <v>569</v>
+        <v>82</v>
       </c>
       <c r="AA92" t="s" s="2">
         <v>82</v>
@@ -13433,7 +13413,7 @@
         <v>82</v>
       </c>
       <c r="AF92" t="s" s="2">
-        <v>570</v>
+        <v>593</v>
       </c>
       <c r="AG92" t="s" s="2">
         <v>80</v>
@@ -13454,10 +13434,10 @@
         <v>82</v>
       </c>
       <c r="AM92" t="s" s="2">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="AN92" t="s" s="2">
-        <v>572</v>
+        <v>594</v>
       </c>
       <c r="AO92" t="s" s="2">
         <v>82</v>
@@ -13468,10 +13448,10 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>574</v>
+        <v>522</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -13479,32 +13459,34 @@
       </c>
       <c r="E93" s="2"/>
       <c r="F93" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G93" t="s" s="2">
         <v>92</v>
       </c>
       <c r="H93" t="s" s="2">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="I93" t="s" s="2">
         <v>82</v>
       </c>
       <c r="J93" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>575</v>
+        <v>523</v>
       </c>
       <c r="M93" t="s" s="2">
-        <v>576</v>
-      </c>
-      <c r="N93" s="2"/>
+        <v>524</v>
+      </c>
+      <c r="N93" t="s" s="2">
+        <v>525</v>
+      </c>
       <c r="O93" t="s" s="2">
-        <v>577</v>
+        <v>370</v>
       </c>
       <c r="P93" t="s" s="2">
         <v>82</v>
@@ -13529,13 +13511,13 @@
         <v>82</v>
       </c>
       <c r="X93" t="s" s="2">
-        <v>82</v>
+        <v>371</v>
       </c>
       <c r="Y93" t="s" s="2">
-        <v>82</v>
+        <v>372</v>
       </c>
       <c r="Z93" t="s" s="2">
-        <v>82</v>
+        <v>373</v>
       </c>
       <c r="AA93" t="s" s="2">
         <v>82</v>
@@ -13553,7 +13535,7 @@
         <v>82</v>
       </c>
       <c r="AF93" t="s" s="2">
-        <v>578</v>
+        <v>522</v>
       </c>
       <c r="AG93" t="s" s="2">
         <v>80</v>
@@ -13562,7 +13544,7 @@
         <v>92</v>
       </c>
       <c r="AI93" t="s" s="2">
-        <v>82</v>
+        <v>526</v>
       </c>
       <c r="AJ93" t="s" s="2">
         <v>104</v>
@@ -13574,10 +13556,10 @@
         <v>82</v>
       </c>
       <c r="AM93" t="s" s="2">
-        <v>579</v>
+        <v>135</v>
       </c>
       <c r="AN93" t="s" s="2">
-        <v>580</v>
+        <v>375</v>
       </c>
       <c r="AO93" t="s" s="2">
         <v>82</v>
@@ -13588,21 +13570,21 @@
     </row>
     <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>582</v>
+        <v>527</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" t="s" s="2">
-        <v>82</v>
+        <v>377</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G94" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H94" t="s" s="2">
         <v>82</v>
@@ -13611,27 +13593,29 @@
         <v>82</v>
       </c>
       <c r="J94" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K94" t="s" s="2">
-        <v>106</v>
+        <v>190</v>
       </c>
       <c r="L94" t="s" s="2">
-        <v>583</v>
+        <v>378</v>
       </c>
       <c r="M94" t="s" s="2">
-        <v>584</v>
-      </c>
-      <c r="N94" s="2"/>
+        <v>379</v>
+      </c>
+      <c r="N94" t="s" s="2">
+        <v>380</v>
+      </c>
       <c r="O94" t="s" s="2">
-        <v>585</v>
+        <v>381</v>
       </c>
       <c r="P94" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q94" s="2"/>
       <c r="R94" t="s" s="2">
-        <v>586</v>
+        <v>82</v>
       </c>
       <c r="S94" t="s" s="2">
         <v>82</v>
@@ -13649,13 +13633,13 @@
         <v>82</v>
       </c>
       <c r="X94" t="s" s="2">
-        <v>82</v>
+        <v>371</v>
       </c>
       <c r="Y94" t="s" s="2">
-        <v>82</v>
+        <v>382</v>
       </c>
       <c r="Z94" t="s" s="2">
-        <v>82</v>
+        <v>383</v>
       </c>
       <c r="AA94" t="s" s="2">
         <v>82</v>
@@ -13673,16 +13657,16 @@
         <v>82</v>
       </c>
       <c r="AF94" t="s" s="2">
-        <v>587</v>
+        <v>527</v>
       </c>
       <c r="AG94" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH94" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI94" t="s" s="2">
-        <v>588</v>
+        <v>82</v>
       </c>
       <c r="AJ94" t="s" s="2">
         <v>104</v>
@@ -13691,27 +13675,27 @@
         <v>82</v>
       </c>
       <c r="AL94" t="s" s="2">
-        <v>82</v>
+        <v>384</v>
       </c>
       <c r="AM94" t="s" s="2">
-        <v>579</v>
+        <v>385</v>
       </c>
       <c r="AN94" t="s" s="2">
-        <v>589</v>
+        <v>386</v>
       </c>
       <c r="AO94" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP94" t="s" s="2">
-        <v>82</v>
+        <v>387</v>
       </c>
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B95" t="s" s="2">
-        <v>591</v>
+        <v>528</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" t="s" s="2">
@@ -13719,10 +13703,10 @@
       </c>
       <c r="E95" s="2"/>
       <c r="F95" t="s" s="2">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="G95" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H95" t="s" s="2">
         <v>82</v>
@@ -13731,29 +13715,29 @@
         <v>82</v>
       </c>
       <c r="J95" t="s" s="2">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="K95" t="s" s="2">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>592</v>
+        <v>529</v>
       </c>
       <c r="M95" t="s" s="2">
-        <v>593</v>
+        <v>530</v>
       </c>
       <c r="N95" t="s" s="2">
-        <v>594</v>
+        <v>437</v>
       </c>
       <c r="O95" t="s" s="2">
-        <v>595</v>
+        <v>438</v>
       </c>
       <c r="P95" t="s" s="2">
         <v>82</v>
       </c>
       <c r="Q95" s="2"/>
       <c r="R95" t="s" s="2">
-        <v>596</v>
+        <v>82</v>
       </c>
       <c r="S95" t="s" s="2">
         <v>82</v>
@@ -13795,13 +13779,13 @@
         <v>82</v>
       </c>
       <c r="AF95" t="s" s="2">
-        <v>597</v>
+        <v>528</v>
       </c>
       <c r="AG95" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AH95" t="s" s="2">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="AI95" t="s" s="2">
         <v>82</v>
@@ -13816,508 +13800,20 @@
         <v>82</v>
       </c>
       <c r="AM95" t="s" s="2">
-        <v>579</v>
+        <v>440</v>
       </c>
       <c r="AN95" t="s" s="2">
-        <v>598</v>
+        <v>441</v>
       </c>
       <c r="AO95" t="s" s="2">
         <v>82</v>
       </c>
       <c r="AP95" t="s" s="2">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="96" hidden="true">
-      <c r="A96" t="s" s="2">
-        <v>611</v>
-      </c>
-      <c r="B96" t="s" s="2">
-        <v>517</v>
-      </c>
-      <c r="C96" s="2"/>
-      <c r="D96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="E96" s="2"/>
-      <c r="F96" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="G96" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="H96" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="I96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="J96" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="K96" t="s" s="2">
-        <v>356</v>
-      </c>
-      <c r="L96" t="s" s="2">
-        <v>518</v>
-      </c>
-      <c r="M96" t="s" s="2">
-        <v>519</v>
-      </c>
-      <c r="N96" t="s" s="2">
-        <v>520</v>
-      </c>
-      <c r="O96" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="P96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Q96" s="2"/>
-      <c r="R96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="S96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="T96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="U96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="V96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="W96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="X96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Y96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Z96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AA96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AB96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AC96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AD96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AE96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AF96" t="s" s="2">
-        <v>517</v>
-      </c>
-      <c r="AG96" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH96" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="AI96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AJ96" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="AK96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AL96" t="s" s="2">
-        <v>521</v>
-      </c>
-      <c r="AM96" t="s" s="2">
-        <v>363</v>
-      </c>
-      <c r="AN96" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="AO96" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AP96" t="s" s="2">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="97" hidden="true">
-      <c r="A97" t="s" s="2">
-        <v>621</v>
-      </c>
-      <c r="B97" t="s" s="2">
-        <v>522</v>
-      </c>
-      <c r="C97" s="2"/>
-      <c r="D97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="E97" s="2"/>
-      <c r="F97" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="G97" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="H97" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="I97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="J97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="K97" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="L97" t="s" s="2">
-        <v>523</v>
-      </c>
-      <c r="M97" t="s" s="2">
-        <v>524</v>
-      </c>
-      <c r="N97" t="s" s="2">
-        <v>525</v>
-      </c>
-      <c r="O97" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="P97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Q97" s="2"/>
-      <c r="R97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="S97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="T97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="U97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="V97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="W97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="X97" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="Y97" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="Z97" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="AA97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AB97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AC97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AD97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AE97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AF97" t="s" s="2">
-        <v>522</v>
-      </c>
-      <c r="AG97" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH97" t="s" s="2">
-        <v>92</v>
-      </c>
-      <c r="AI97" t="s" s="2">
-        <v>526</v>
-      </c>
-      <c r="AJ97" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="AK97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AL97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AM97" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="AN97" t="s" s="2">
-        <v>375</v>
-      </c>
-      <c r="AO97" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AP97" t="s" s="2">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="98" hidden="true">
-      <c r="A98" t="s" s="2">
-        <v>622</v>
-      </c>
-      <c r="B98" t="s" s="2">
-        <v>527</v>
-      </c>
-      <c r="C98" s="2"/>
-      <c r="D98" t="s" s="2">
-        <v>377</v>
-      </c>
-      <c r="E98" s="2"/>
-      <c r="F98" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="G98" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="H98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="I98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="J98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="K98" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="L98" t="s" s="2">
-        <v>378</v>
-      </c>
-      <c r="M98" t="s" s="2">
-        <v>379</v>
-      </c>
-      <c r="N98" t="s" s="2">
-        <v>380</v>
-      </c>
-      <c r="O98" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="P98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Q98" s="2"/>
-      <c r="R98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="S98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="T98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="U98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="V98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="W98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="X98" t="s" s="2">
-        <v>371</v>
-      </c>
-      <c r="Y98" t="s" s="2">
-        <v>382</v>
-      </c>
-      <c r="Z98" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="AA98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AB98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AC98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AD98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AE98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AF98" t="s" s="2">
-        <v>527</v>
-      </c>
-      <c r="AG98" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH98" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AJ98" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="AK98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AL98" t="s" s="2">
-        <v>384</v>
-      </c>
-      <c r="AM98" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="AN98" t="s" s="2">
-        <v>386</v>
-      </c>
-      <c r="AO98" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AP98" t="s" s="2">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="99" hidden="true">
-      <c r="A99" t="s" s="2">
-        <v>623</v>
-      </c>
-      <c r="B99" t="s" s="2">
-        <v>528</v>
-      </c>
-      <c r="C99" s="2"/>
-      <c r="D99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="E99" s="2"/>
-      <c r="F99" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="G99" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="H99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="I99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="J99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="K99" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="L99" t="s" s="2">
-        <v>529</v>
-      </c>
-      <c r="M99" t="s" s="2">
-        <v>530</v>
-      </c>
-      <c r="N99" t="s" s="2">
-        <v>437</v>
-      </c>
-      <c r="O99" t="s" s="2">
-        <v>438</v>
-      </c>
-      <c r="P99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Q99" s="2"/>
-      <c r="R99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="S99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="T99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="U99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="V99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="W99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="X99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Y99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="Z99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AA99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AB99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AC99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AD99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AE99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AF99" t="s" s="2">
-        <v>528</v>
-      </c>
-      <c r="AG99" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AH99" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="AI99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AJ99" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="AK99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AL99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AM99" t="s" s="2">
-        <v>440</v>
-      </c>
-      <c r="AN99" t="s" s="2">
-        <v>441</v>
-      </c>
-      <c r="AO99" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="AP99" t="s" s="2">
         <v>82</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP99">
+  <autoFilter ref="A1:AP95">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -14327,7 +13823,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI98">
+  <conditionalFormatting sqref="A2:AI94">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>